<commit_message>
iteration 1 documents update
</commit_message>
<xml_diff>
--- a/doc/CS673_ProgressReport_team3.xlsx
+++ b/doc/CS673_ProgressReport_team3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="238">
   <si>
     <t xml:space="preserve">This report has 1 group iteration progress summary sheet to be filled at the end of each iteration by the team leader, 
 1 project ontribution sheet to be filled by everyone at the end of the semester, and 1 weekly report sheet per student. </t>
@@ -1530,8 +1530,101 @@
   </si>
   <si>
     <t>0 - learn expo, RN, RN web
-5 - attended project meeting and documented meeting notes.
-6 - set up coding environment</t>
+2 - design Game1 structure and constants
+3 - import outer libraries to help render
+5 - discuss the AI usage possibilities for UI
+6 - configure build environment and fix import / module errors when running outside libraries</t>
+  </si>
+  <si>
+    <t>Used ChatGPT to understand how to call outside libraries that help render game from React Native, including import path setup and module export adjustment. Helpful for resolving bundler and rendering issues.</t>
+  </si>
+  <si>
+    <t>1. Setup Game1 branch
+2. Completed GameMenu basic layout and navigation structure.
+3. Verified screen transition logic between Home and GameMenu.
+4. Configured and tested Expo development environment for React Native and web platforms.</t>
+  </si>
+  <si>
+    <t>1. Laptop Broken :(
+2. Expo startup failure and persistent blank screen on both simulator and web preview.
+3. Environment mismatch between React version and installed dependencies.</t>
+  </si>
+  <si>
+    <t>Solved
+1. Buy a new one
+2. Reinstalled and reconfigured Expo CLI and React 19 environment
+3. Cleared cache, rebuilt node_modules, and verified compatibility
+4. Confirmed GameMenu running successfully on simulator and web after fix.</t>
+  </si>
+  <si>
+    <t>0 - Learn how to implement and render inside React directly
+2 - Design more games
+3 - Finish the implementation of Game1
+7 - Finished Lab2 documents</t>
+  </si>
+  <si>
+    <t>0 - research how to integrate helper libraries into React Native environment
+3 - implement player movement, gravity, and jump mechanics, implement collision detection, player controls, and scoring system
+4 - manual test Game1 gameplay, including win and lose conditions, test rendering across devices
+5 - discuss UI consistency, discuss platform and environment usage
+6 - debug import and module errors</t>
+  </si>
+  <si>
+    <t>Used ChatGPT to help understand and render the game and animation inside React Native. Helpful since import outside helper libraries is nearly impossible, solve the render problem.</t>
+  </si>
+  <si>
+    <t>1. Designed Game1 (GolfMe) structure and gameplay constants (gravity, jump, scroll).
+2. Tested performance on web and Android.
+3. Maintained visual consistency with layout.</t>
+  </si>
+  <si>
+    <t>1. Import failure due to ESM module path issue.
+2. The game ratio is strange and screen is black
+3. Gameplay speed inconsistency across devices.
+4. Expo hot reload crash during game script execution.</t>
+  </si>
+  <si>
+    <t>Solved
+1. Used AI to instead the import methods
+2. Adjusted gravity and frame update rate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 - Design game 2 gameplay
+3 - Integrate reusable components and scoring
+4 - Automatic test and Unit test for games, also the CI/CD
+7 - Finish iteration 1
+</t>
+  </si>
+  <si>
+    <t>2 - refine UI design for Game1, design Game2 structure and constants
+3 - complete Game2 implementation with core logic and gameplay loop
+4 - conduct detailed multi-device testing (Game1 &amp; Game2) focusing on performance and rendering
+5 - discuss further functionalities, and some restrictions for game part to make it suitable for our app
+6 - fix React Native runtime warnings and optimize code structure</t>
+  </si>
+  <si>
+    <t>Used ChatGPT to investigate why several test cases always failed, including version mismatch between React Native and Expo SDK. Also used it to check dependency compatibility, rebuild environment, and analyze logs from failed runs. Very helpful for environment diagnosis and test debugging.</t>
+  </si>
+  <si>
+    <t>1. Completed Game2 gameplay logic using React Native physics and event system.
+2. Improved scoring accuracy and collision stability.
+3. Conducted detailed manual cross-platform testing on web, iOS, and Android.
+4. Identified and documented unsolved test failures and runtime inconsistencies.
+5. Key algorithms part in SDD file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Environment conflict: mismatch between React 19, Expo SDK 52, and React Navigation version.
+2. Testing configuration issue: serious incompatibility between Babel, Vitest, and Jest in handling React 19 JSX transforms.
+3. The transpilation flow cannot be properly transferred — Babel compiles JSX for Metro bundler, while Vitest reprocesses the same files with different ESM rules, and Jest expects CommonJS modules. As a result, test runs failed to import components correctly, producing “Unexpected token import/export” and “Cannot use import statement outside a module” errors.
+</t>
+  </si>
+  <si>
+    <t>Unsolved
+1. Shinu said this may be fixed since there was a recent hotfix for this, try next week</t>
+  </si>
+  <si>
+    <t>2 - design another 3 games
+3 - time restrictions for users who enter the game menu, and rewards for high scores</t>
   </si>
 </sst>
 </file>
@@ -2236,11 +2329,11 @@
       </c>
       <c r="L5" s="10">
         <f>'Melissa Cron'!C5+'Melissa Cron'!C6+'Melissa Cron'!C7+'Dexiao Zhang'!C6+'Dexiao Zhang'!C7+'Dexiao Zhang'!C8+'Junzhe Chen'!C5+'Junzhe Chen'!C6+'Ittoop Shinu Shibu'!C5+'Ittoop Shinu Shibu'!C6+'Ittoop Shinu Shibu'!C7+'Bohan Lin'!C5+'Bohan Lin'!C6+'Bohan Lin'!C7+'Qiuting Zhao'!C5+'Qiuting Zhao'!C6+'Qiuting Zhao'!C7</f>
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="M5" s="10">
         <f>'Melissa Cron'!D5+'Melissa Cron'!D6+'Melissa Cron'!D7+'Dexiao Zhang'!D6+'Dexiao Zhang'!D7+'Dexiao Zhang'!D8+'Junzhe Chen'!D5+'Junzhe Chen'!D6+'Ittoop Shinu Shibu'!D5+'Ittoop Shinu Shibu'!D6+'Ittoop Shinu Shibu'!D7+'Bohan Lin'!D5+'Bohan Lin'!D6+'Bohan Lin'!D7+'Qiuting Zhao'!D5+'Qiuting Zhao'!D6+'Qiuting Zhao'!D7</f>
-        <v>254</v>
+        <v>298</v>
       </c>
       <c r="N5" s="10">
         <f>'Melissa Cron'!E5+'Melissa Cron'!E6+'Melissa Cron'!E7+'Dexiao Zhang'!E6+'Dexiao Zhang'!E7+'Dexiao Zhang'!E8+'Junzhe Chen'!E5+'Junzhe Chen'!E6+'Ittoop Shinu Shibu'!E5+'Ittoop Shinu Shibu'!E6+'Ittoop Shinu Shibu'!E7+'Bohan Lin'!E5+'Bohan Lin'!E6+'Bohan Lin'!E7+'Qiuting Zhao'!E5+'Qiuting Zhao'!E6+'Qiuting Zhao'!E7</f>
@@ -2248,31 +2341,31 @@
       </c>
       <c r="O5" s="10">
         <f>'Melissa Cron'!G5+'Melissa Cron'!G6+'Melissa Cron'!G7+'Dexiao Zhang'!G6+'Dexiao Zhang'!G7+'Dexiao Zhang'!G8+'Junzhe Chen'!G5+'Junzhe Chen'!G6+'Ittoop Shinu Shibu'!G5+'Ittoop Shinu Shibu'!G6+'Ittoop Shinu Shibu'!G7+'Bohan Lin'!G5+'Bohan Lin'!G6+'Bohan Lin'!G7+'Qiuting Zhao'!G5+'Qiuting Zhao'!G6+'Qiuting Zhao'!G7</f>
-        <v>36</v>
+        <v>32.5</v>
       </c>
       <c r="P5" s="10">
         <f>'Melissa Cron'!H5+'Melissa Cron'!H6+'Melissa Cron'!H7+'Dexiao Zhang'!H6+'Dexiao Zhang'!H7+'Dexiao Zhang'!H8+'Junzhe Chen'!H5+'Junzhe Chen'!H6+'Ittoop Shinu Shibu'!H5+'Ittoop Shinu Shibu'!H6+'Ittoop Shinu Shibu'!H7+'Bohan Lin'!H5+'Bohan Lin'!H6+'Bohan Lin'!H7+'Qiuting Zhao'!H5+'Qiuting Zhao'!H6+'Qiuting Zhao'!H7</f>
-        <v>25</v>
+        <v>23.5</v>
       </c>
       <c r="Q5" s="10">
         <f>'Melissa Cron'!I5+'Melissa Cron'!I6+'Melissa Cron'!I7+'Dexiao Zhang'!I6+'Dexiao Zhang'!I7+'Dexiao Zhang'!I8+'Junzhe Chen'!I5+'Junzhe Chen'!I6+'Ittoop Shinu Shibu'!I5+'Ittoop Shinu Shibu'!I6+'Ittoop Shinu Shibu'!I7+'Bohan Lin'!I5+'Bohan Lin'!I6+'Bohan Lin'!I7+'Qiuting Zhao'!I5+'Qiuting Zhao'!I6+'Qiuting Zhao'!I7</f>
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="R5" s="10">
         <f>'Melissa Cron'!J5+'Melissa Cron'!J6+'Melissa Cron'!J7+'Dexiao Zhang'!J6+'Dexiao Zhang'!J7+'Dexiao Zhang'!J8+'Junzhe Chen'!J5+'Junzhe Chen'!J6+'Ittoop Shinu Shibu'!J5+'Ittoop Shinu Shibu'!J6+'Ittoop Shinu Shibu'!J7+'Bohan Lin'!J5+'Bohan Lin'!J6+'Bohan Lin'!J7+'Qiuting Zhao'!J5+'Qiuting Zhao'!J6+'Qiuting Zhao'!J7</f>
-        <v>55.5</v>
+        <v>70.5</v>
       </c>
       <c r="S5" s="10">
         <f>'Melissa Cron'!K5+'Melissa Cron'!K6+'Melissa Cron'!K7+'Dexiao Zhang'!K6+'Dexiao Zhang'!K7+'Dexiao Zhang'!K8+'Junzhe Chen'!K5+'Junzhe Chen'!K6+'Ittoop Shinu Shibu'!K5+'Ittoop Shinu Shibu'!K6+'Ittoop Shinu Shibu'!K7+'Bohan Lin'!K5+'Bohan Lin'!K6+'Bohan Lin'!K7+'Qiuting Zhao'!K5+'Qiuting Zhao'!K6+'Qiuting Zhao'!K7</f>
-        <v>23.5</v>
+        <v>37.5</v>
       </c>
       <c r="T5" s="10">
         <f>'Melissa Cron'!L5+'Melissa Cron'!L6+'Melissa Cron'!L7+'Dexiao Zhang'!L6+'Dexiao Zhang'!L7+'Dexiao Zhang'!L8+'Junzhe Chen'!L5+'Junzhe Chen'!L6+'Ittoop Shinu Shibu'!L5+'Ittoop Shinu Shibu'!L6+'Ittoop Shinu Shibu'!L7+'Bohan Lin'!L5+'Bohan Lin'!L6+'Bohan Lin'!L7+'Qiuting Zhao'!L5+'Qiuting Zhao'!L6+'Qiuting Zhao'!L7</f>
-        <v>16</v>
+        <v>16.5</v>
       </c>
       <c r="U5" s="10">
         <f>'Melissa Cron'!M5+'Melissa Cron'!M6+'Melissa Cron'!M7+'Dexiao Zhang'!M6+'Dexiao Zhang'!M7+'Dexiao Zhang'!M8+'Junzhe Chen'!M5+'Junzhe Chen'!M6+'Ittoop Shinu Shibu'!M5+'Ittoop Shinu Shibu'!M6+'Ittoop Shinu Shibu'!M7+'Bohan Lin'!M5+'Bohan Lin'!M6+'Bohan Lin'!M7+'Qiuting Zhao'!M5+'Qiuting Zhao'!M6+'Qiuting Zhao'!M7</f>
-        <v>53</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="6">
@@ -58028,11 +58121,11 @@
       </c>
       <c r="C5" s="24">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>17.5</v>
       </c>
       <c r="D5" s="24">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>16.5</v>
       </c>
       <c r="E5" s="7">
         <v>1.0</v>
@@ -58040,39 +58133,43 @@
       <c r="F5" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="G5" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="J5" s="34">
+        <v>4.0</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <v>1.0</v>
       </c>
-      <c r="M5" s="7">
-        <v>1.0</v>
+      <c r="M5" s="34">
+        <v>8.0</v>
       </c>
       <c r="N5" s="7"/>
-      <c r="O5" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="T5" s="7">
-        <v>10.0</v>
+      <c r="O5" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="T5" s="34">
+        <v>20.0</v>
       </c>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
@@ -58091,49 +58188,53 @@
       </c>
       <c r="C6" s="24">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>19</v>
       </c>
       <c r="D6" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>17.5</v>
       </c>
       <c r="E6" s="34">
         <v>1.5</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="G6" s="6">
-        <v>2.5</v>
+      <c r="F6" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3.5</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6">
+      <c r="J6" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="L6" s="8">
         <v>1.0</v>
       </c>
-      <c r="M6" s="6">
-        <v>0.5</v>
+      <c r="M6" s="8">
+        <v>4.0</v>
       </c>
       <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="T6" s="6">
-        <v>10.0</v>
+      <c r="O6" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="T6" s="8">
+        <v>25.0</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -58148,49 +58249,53 @@
       </c>
       <c r="C7" s="24">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>31.5</v>
       </c>
       <c r="D7" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>30.5</v>
       </c>
       <c r="E7" s="34">
         <v>1.0</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="F7" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="J7" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="M7" s="8">
         <v>2.5</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0.5</v>
-      </c>
       <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="T7" s="6">
-        <v>10.0</v>
+      <c r="O7" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="T7" s="8">
+        <v>30.0</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>

</xml_diff>

<commit_message>
Bump tar from 7.5.1 to 7.5.2 in /code/Study buddy/frontend (#33)
* iteration 1 documents update

* Bump tar from 7.5.1 to 7.5.2 in /code/Study buddy/frontend

Bumps [tar](https://github.com/isaacs/node-tar) from 7.5.1 to 7.5.2.
- [Release notes](https://github.com/isaacs/node-tar/releases)
- [Changelog](https://github.com/isaacs/node-tar/blob/main/CHANGELOG.md)
- [Commits](https://github.com/isaacs/node-tar/compare/v7.5.1...v7.5.2)

---
updated-dependencies:
- dependency-name: tar
  dependency-version: 7.5.2
  dependency-type: indirect
...

Signed-off-by: dependabot[bot] <support@github.com>

---------

Signed-off-by: dependabot[bot] <support@github.com>
Co-authored-by: shinushibu1798 <31847296+shinushibu1798@users.noreply.github.com>
Co-authored-by: QtinzIa <qtin28@gmail.com>
Co-authored-by: QtinzIa <86401155+QtinzIa@users.noreply.github.com>
Co-authored-by: dependabot[bot] <49699333+dependabot[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/doc/CS673_ProgressReport_team3.xlsx
+++ b/doc/CS673_ProgressReport_team3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="238">
   <si>
     <t xml:space="preserve">This report has 1 group iteration progress summary sheet to be filled at the end of each iteration by the team leader, 
 1 project ontribution sheet to be filled by everyone at the end of the semester, and 1 weekly report sheet per student. </t>
@@ -1530,8 +1530,101 @@
   </si>
   <si>
     <t>0 - learn expo, RN, RN web
-5 - attended project meeting and documented meeting notes.
-6 - set up coding environment</t>
+2 - design Game1 structure and constants
+3 - import outer libraries to help render
+5 - discuss the AI usage possibilities for UI
+6 - configure build environment and fix import / module errors when running outside libraries</t>
+  </si>
+  <si>
+    <t>Used ChatGPT to understand how to call outside libraries that help render game from React Native, including import path setup and module export adjustment. Helpful for resolving bundler and rendering issues.</t>
+  </si>
+  <si>
+    <t>1. Setup Game1 branch
+2. Completed GameMenu basic layout and navigation structure.
+3. Verified screen transition logic between Home and GameMenu.
+4. Configured and tested Expo development environment for React Native and web platforms.</t>
+  </si>
+  <si>
+    <t>1. Laptop Broken :(
+2. Expo startup failure and persistent blank screen on both simulator and web preview.
+3. Environment mismatch between React version and installed dependencies.</t>
+  </si>
+  <si>
+    <t>Solved
+1. Buy a new one
+2. Reinstalled and reconfigured Expo CLI and React 19 environment
+3. Cleared cache, rebuilt node_modules, and verified compatibility
+4. Confirmed GameMenu running successfully on simulator and web after fix.</t>
+  </si>
+  <si>
+    <t>0 - Learn how to implement and render inside React directly
+2 - Design more games
+3 - Finish the implementation of Game1
+7 - Finished Lab2 documents</t>
+  </si>
+  <si>
+    <t>0 - research how to integrate helper libraries into React Native environment
+3 - implement player movement, gravity, and jump mechanics, implement collision detection, player controls, and scoring system
+4 - manual test Game1 gameplay, including win and lose conditions, test rendering across devices
+5 - discuss UI consistency, discuss platform and environment usage
+6 - debug import and module errors</t>
+  </si>
+  <si>
+    <t>Used ChatGPT to help understand and render the game and animation inside React Native. Helpful since import outside helper libraries is nearly impossible, solve the render problem.</t>
+  </si>
+  <si>
+    <t>1. Designed Game1 (GolfMe) structure and gameplay constants (gravity, jump, scroll).
+2. Tested performance on web and Android.
+3. Maintained visual consistency with layout.</t>
+  </si>
+  <si>
+    <t>1. Import failure due to ESM module path issue.
+2. The game ratio is strange and screen is black
+3. Gameplay speed inconsistency across devices.
+4. Expo hot reload crash during game script execution.</t>
+  </si>
+  <si>
+    <t>Solved
+1. Used AI to instead the import methods
+2. Adjusted gravity and frame update rate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 - Design game 2 gameplay
+3 - Integrate reusable components and scoring
+4 - Automatic test and Unit test for games, also the CI/CD
+7 - Finish iteration 1
+</t>
+  </si>
+  <si>
+    <t>2 - refine UI design for Game1, design Game2 structure and constants
+3 - complete Game2 implementation with core logic and gameplay loop
+4 - conduct detailed multi-device testing (Game1 &amp; Game2) focusing on performance and rendering
+5 - discuss further functionalities, and some restrictions for game part to make it suitable for our app
+6 - fix React Native runtime warnings and optimize code structure</t>
+  </si>
+  <si>
+    <t>Used ChatGPT to investigate why several test cases always failed, including version mismatch between React Native and Expo SDK. Also used it to check dependency compatibility, rebuild environment, and analyze logs from failed runs. Very helpful for environment diagnosis and test debugging.</t>
+  </si>
+  <si>
+    <t>1. Completed Game2 gameplay logic using React Native physics and event system.
+2. Improved scoring accuracy and collision stability.
+3. Conducted detailed manual cross-platform testing on web, iOS, and Android.
+4. Identified and documented unsolved test failures and runtime inconsistencies.
+5. Key algorithms part in SDD file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Environment conflict: mismatch between React 19, Expo SDK 52, and React Navigation version.
+2. Testing configuration issue: serious incompatibility between Babel, Vitest, and Jest in handling React 19 JSX transforms.
+3. The transpilation flow cannot be properly transferred — Babel compiles JSX for Metro bundler, while Vitest reprocesses the same files with different ESM rules, and Jest expects CommonJS modules. As a result, test runs failed to import components correctly, producing “Unexpected token import/export” and “Cannot use import statement outside a module” errors.
+</t>
+  </si>
+  <si>
+    <t>Unsolved
+1. Shinu said this may be fixed since there was a recent hotfix for this, try next week</t>
+  </si>
+  <si>
+    <t>2 - design another 3 games
+3 - time restrictions for users who enter the game menu, and rewards for high scores</t>
   </si>
 </sst>
 </file>
@@ -2236,11 +2329,11 @@
       </c>
       <c r="L5" s="10">
         <f>'Melissa Cron'!C5+'Melissa Cron'!C6+'Melissa Cron'!C7+'Dexiao Zhang'!C6+'Dexiao Zhang'!C7+'Dexiao Zhang'!C8+'Junzhe Chen'!C5+'Junzhe Chen'!C6+'Ittoop Shinu Shibu'!C5+'Ittoop Shinu Shibu'!C6+'Ittoop Shinu Shibu'!C7+'Bohan Lin'!C5+'Bohan Lin'!C6+'Bohan Lin'!C7+'Qiuting Zhao'!C5+'Qiuting Zhao'!C6+'Qiuting Zhao'!C7</f>
-        <v>274</v>
+        <v>318</v>
       </c>
       <c r="M5" s="10">
         <f>'Melissa Cron'!D5+'Melissa Cron'!D6+'Melissa Cron'!D7+'Dexiao Zhang'!D6+'Dexiao Zhang'!D7+'Dexiao Zhang'!D8+'Junzhe Chen'!D5+'Junzhe Chen'!D6+'Ittoop Shinu Shibu'!D5+'Ittoop Shinu Shibu'!D6+'Ittoop Shinu Shibu'!D7+'Bohan Lin'!D5+'Bohan Lin'!D6+'Bohan Lin'!D7+'Qiuting Zhao'!D5+'Qiuting Zhao'!D6+'Qiuting Zhao'!D7</f>
-        <v>254</v>
+        <v>298</v>
       </c>
       <c r="N5" s="10">
         <f>'Melissa Cron'!E5+'Melissa Cron'!E6+'Melissa Cron'!E7+'Dexiao Zhang'!E6+'Dexiao Zhang'!E7+'Dexiao Zhang'!E8+'Junzhe Chen'!E5+'Junzhe Chen'!E6+'Ittoop Shinu Shibu'!E5+'Ittoop Shinu Shibu'!E6+'Ittoop Shinu Shibu'!E7+'Bohan Lin'!E5+'Bohan Lin'!E6+'Bohan Lin'!E7+'Qiuting Zhao'!E5+'Qiuting Zhao'!E6+'Qiuting Zhao'!E7</f>
@@ -2248,31 +2341,31 @@
       </c>
       <c r="O5" s="10">
         <f>'Melissa Cron'!G5+'Melissa Cron'!G6+'Melissa Cron'!G7+'Dexiao Zhang'!G6+'Dexiao Zhang'!G7+'Dexiao Zhang'!G8+'Junzhe Chen'!G5+'Junzhe Chen'!G6+'Ittoop Shinu Shibu'!G5+'Ittoop Shinu Shibu'!G6+'Ittoop Shinu Shibu'!G7+'Bohan Lin'!G5+'Bohan Lin'!G6+'Bohan Lin'!G7+'Qiuting Zhao'!G5+'Qiuting Zhao'!G6+'Qiuting Zhao'!G7</f>
-        <v>36</v>
+        <v>32.5</v>
       </c>
       <c r="P5" s="10">
         <f>'Melissa Cron'!H5+'Melissa Cron'!H6+'Melissa Cron'!H7+'Dexiao Zhang'!H6+'Dexiao Zhang'!H7+'Dexiao Zhang'!H8+'Junzhe Chen'!H5+'Junzhe Chen'!H6+'Ittoop Shinu Shibu'!H5+'Ittoop Shinu Shibu'!H6+'Ittoop Shinu Shibu'!H7+'Bohan Lin'!H5+'Bohan Lin'!H6+'Bohan Lin'!H7+'Qiuting Zhao'!H5+'Qiuting Zhao'!H6+'Qiuting Zhao'!H7</f>
-        <v>25</v>
+        <v>23.5</v>
       </c>
       <c r="Q5" s="10">
         <f>'Melissa Cron'!I5+'Melissa Cron'!I6+'Melissa Cron'!I7+'Dexiao Zhang'!I6+'Dexiao Zhang'!I7+'Dexiao Zhang'!I8+'Junzhe Chen'!I5+'Junzhe Chen'!I6+'Ittoop Shinu Shibu'!I5+'Ittoop Shinu Shibu'!I6+'Ittoop Shinu Shibu'!I7+'Bohan Lin'!I5+'Bohan Lin'!I6+'Bohan Lin'!I7+'Qiuting Zhao'!I5+'Qiuting Zhao'!I6+'Qiuting Zhao'!I7</f>
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="R5" s="10">
         <f>'Melissa Cron'!J5+'Melissa Cron'!J6+'Melissa Cron'!J7+'Dexiao Zhang'!J6+'Dexiao Zhang'!J7+'Dexiao Zhang'!J8+'Junzhe Chen'!J5+'Junzhe Chen'!J6+'Ittoop Shinu Shibu'!J5+'Ittoop Shinu Shibu'!J6+'Ittoop Shinu Shibu'!J7+'Bohan Lin'!J5+'Bohan Lin'!J6+'Bohan Lin'!J7+'Qiuting Zhao'!J5+'Qiuting Zhao'!J6+'Qiuting Zhao'!J7</f>
-        <v>55.5</v>
+        <v>70.5</v>
       </c>
       <c r="S5" s="10">
         <f>'Melissa Cron'!K5+'Melissa Cron'!K6+'Melissa Cron'!K7+'Dexiao Zhang'!K6+'Dexiao Zhang'!K7+'Dexiao Zhang'!K8+'Junzhe Chen'!K5+'Junzhe Chen'!K6+'Ittoop Shinu Shibu'!K5+'Ittoop Shinu Shibu'!K6+'Ittoop Shinu Shibu'!K7+'Bohan Lin'!K5+'Bohan Lin'!K6+'Bohan Lin'!K7+'Qiuting Zhao'!K5+'Qiuting Zhao'!K6+'Qiuting Zhao'!K7</f>
-        <v>23.5</v>
+        <v>37.5</v>
       </c>
       <c r="T5" s="10">
         <f>'Melissa Cron'!L5+'Melissa Cron'!L6+'Melissa Cron'!L7+'Dexiao Zhang'!L6+'Dexiao Zhang'!L7+'Dexiao Zhang'!L8+'Junzhe Chen'!L5+'Junzhe Chen'!L6+'Ittoop Shinu Shibu'!L5+'Ittoop Shinu Shibu'!L6+'Ittoop Shinu Shibu'!L7+'Bohan Lin'!L5+'Bohan Lin'!L6+'Bohan Lin'!L7+'Qiuting Zhao'!L5+'Qiuting Zhao'!L6+'Qiuting Zhao'!L7</f>
-        <v>16</v>
+        <v>16.5</v>
       </c>
       <c r="U5" s="10">
         <f>'Melissa Cron'!M5+'Melissa Cron'!M6+'Melissa Cron'!M7+'Dexiao Zhang'!M6+'Dexiao Zhang'!M7+'Dexiao Zhang'!M8+'Junzhe Chen'!M5+'Junzhe Chen'!M6+'Ittoop Shinu Shibu'!M5+'Ittoop Shinu Shibu'!M6+'Ittoop Shinu Shibu'!M7+'Bohan Lin'!M5+'Bohan Lin'!M6+'Bohan Lin'!M7+'Qiuting Zhao'!M5+'Qiuting Zhao'!M6+'Qiuting Zhao'!M7</f>
-        <v>53</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="6">
@@ -58028,11 +58121,11 @@
       </c>
       <c r="C5" s="24">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>17.5</v>
       </c>
       <c r="D5" s="24">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>16.5</v>
       </c>
       <c r="E5" s="7">
         <v>1.0</v>
@@ -58040,39 +58133,43 @@
       <c r="F5" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="G5" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="J5" s="34">
+        <v>4.0</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7">
         <v>1.0</v>
       </c>
-      <c r="M5" s="7">
-        <v>1.0</v>
+      <c r="M5" s="34">
+        <v>8.0</v>
       </c>
       <c r="N5" s="7"/>
-      <c r="O5" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="T5" s="7">
-        <v>10.0</v>
+      <c r="O5" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="T5" s="34">
+        <v>20.0</v>
       </c>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
@@ -58091,49 +58188,53 @@
       </c>
       <c r="C6" s="24">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>19</v>
       </c>
       <c r="D6" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>17.5</v>
       </c>
       <c r="E6" s="34">
         <v>1.5</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="G6" s="6">
-        <v>2.5</v>
+      <c r="F6" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3.5</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6">
+      <c r="J6" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="L6" s="8">
         <v>1.0</v>
       </c>
-      <c r="M6" s="6">
-        <v>0.5</v>
+      <c r="M6" s="8">
+        <v>4.0</v>
       </c>
       <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="T6" s="6">
-        <v>10.0</v>
+      <c r="O6" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="T6" s="8">
+        <v>25.0</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -58148,49 +58249,53 @@
       </c>
       <c r="C7" s="24">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>31.5</v>
       </c>
       <c r="D7" s="24">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>30.5</v>
       </c>
       <c r="E7" s="34">
         <v>1.0</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="F7" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="J7" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="M7" s="8">
         <v>2.5</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0.5</v>
-      </c>
       <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="T7" s="6">
-        <v>10.0</v>
+      <c r="O7" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="T7" s="8">
+        <v>30.0</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>

</xml_diff>

<commit_message>
update docs for iteration2
</commit_message>
<xml_diff>
--- a/doc/CS673_ProgressReport_team3.xlsx
+++ b/doc/CS673_ProgressReport_team3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="348">
   <si>
     <t xml:space="preserve">This report has 1 group iteration progress summary sheet to be filled at the end of each iteration by the team leader, 
 1 project ontribution sheet to be filled by everyone at the end of the semester, and 1 weekly report sheet per student. </t>
@@ -2170,10 +2170,20 @@
 7 - Tried to merge develop with frontend_stats branch. Merging failed due to multiple people making changes on the branch. </t>
   </si>
   <si>
+    <t xml:space="preserve">Login frontend screen. </t>
+  </si>
+  <si>
     <t>7 - Initial route debug. Used different branch to merge frontend calendar into develop. Wrote testing metrics on STD file. Update class diagram on SPPP file. Reviewed hotfix pull requet and other pull requests.</t>
   </si>
   <si>
     <t>STD file, SDD file, updated</t>
+  </si>
+  <si>
+    <t>Team members are not reviewing pull requests.</t>
+  </si>
+  <si>
+    <t>status: open
+Communication needed among team members.</t>
   </si>
   <si>
     <r>
@@ -2404,11 +2414,14 @@
   <si>
     <t>1. API_BASE_URL: undefined
 Auth endpoint: undefined/users/login
-Login page does not work on expo</t>
+Login page does not work on expo
+2. Merge and push to wrong branches</t>
   </si>
   <si>
     <t>Unsolved
-1. Suspect wifi problem, try later</t>
+1. Suspect wifi problem, try later
+Solved
+1. Revert wrong PR</t>
   </si>
   <si>
     <t>3 - Design and implement the reward system for game, link the score record to users' databases</t>
@@ -56292,7 +56305,9 @@
         <v>4.0</v>
       </c>
       <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="P9" s="8" t="s">
+        <v>295</v>
+      </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
@@ -56322,7 +56337,7 @@
         <v>1.0</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -56336,10 +56351,14 @@
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
+        <v>297</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>299</v>
+      </c>
       <c r="S10" s="6"/>
       <c r="T10" s="8">
         <v>20.0</v>
@@ -61121,7 +61140,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
@@ -61229,7 +61248,7 @@
         <v>1.0</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="G3" s="7">
         <v>3.0</v>
@@ -61248,19 +61267,19 @@
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="19" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="T3" s="7">
         <v>10.0</v>
@@ -61292,7 +61311,7 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G4" s="6">
         <v>2.5</v>
@@ -61312,16 +61331,16 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="T4" s="6">
         <v>10.0</v>
@@ -61349,7 +61368,7 @@
         <v>1.0</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="G5" s="7">
         <v>1.0</v>
@@ -61372,19 +61391,19 @@
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="19" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="T5" s="7">
         <v>20.0</v>
@@ -61416,7 +61435,7 @@
         <v>1.5</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="G6" s="6">
         <v>3.5</v>
@@ -61437,19 +61456,19 @@
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="T6" s="6">
         <v>25.0</v>
@@ -61477,7 +61496,7 @@
         <v>1.0</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -61498,19 +61517,19 @@
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="T7" s="6">
         <v>30.0</v>
@@ -61538,7 +61557,7 @@
         <v>1.0</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -61559,19 +61578,19 @@
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="28" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="P8" s="28" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="T8" s="8">
         <v>10.0</v>
@@ -61599,7 +61618,7 @@
         <v>1.0</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -61618,19 +61637,19 @@
       <c r="M9" s="8"/>
       <c r="N9" s="6"/>
       <c r="O9" s="28" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="P9" s="28" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="T9" s="8">
         <v>15.0</v>
@@ -61658,7 +61677,7 @@
         <v>0.0</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -61679,19 +61698,19 @@
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="8" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="T10" s="8">
         <v>20.0</v>

</xml_diff>